<commit_message>
1des sop excel modulo add aula11
</commit_message>
<xml_diff>
--- a/1des/sop/aula10/FolhaDePag.xlsx
+++ b/1des/sop/aula10/FolhaDePag.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\1des\sop\aula10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wellington.martins\Desktop\github\senai2021\1des\sop\aula10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="2" r:id="rId1"/>
     <sheet name="Folha2021" sheetId="1" r:id="rId2"/>
-    <sheet name="Plan1" sheetId="3" r:id="rId3"/>
+    <sheet name="SolveProblem" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Folha2021!$B$6:$S$41</definedName>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
   <si>
     <t>Allan Cesar da Silva</t>
   </si>
@@ -472,12 +472,6 @@
     <t>Problema</t>
   </si>
   <si>
-    <t>Tem solução</t>
-  </si>
-  <si>
-    <t>Trivial</t>
-  </si>
-  <si>
     <t>Não tem solução</t>
   </si>
   <si>
@@ -500,6 +494,27 @@
   </si>
   <si>
     <t>Receita, de passos</t>
+  </si>
+  <si>
+    <t>Etapas</t>
+  </si>
+  <si>
+    <t>Solução de</t>
+  </si>
+  <si>
+    <t>Tem solução Trivial</t>
+  </si>
+  <si>
+    <t>Tem solução não Trivial</t>
+  </si>
+  <si>
+    <t>É problema</t>
+  </si>
+  <si>
+    <t>Não é problema</t>
+  </si>
+  <si>
+    <t>O que é problema</t>
   </si>
 </sst>
 </file>
@@ -619,6 +634,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -628,7 +644,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -914,7 +929,7 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -931,20 +946,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="B1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="16"/>
+      <c r="H1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1077,12 +1092,12 @@
       <c r="B9" s="3">
         <v>1558.5</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1173,12 +1188,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -1292,11 +1307,11 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,33 +1336,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -1372,7 +1387,7 @@
       <c r="E5" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="15">
         <v>0.75</v>
       </c>
       <c r="S5" s="14">
@@ -4155,11 +4170,11 @@
       <c r="R45" s="5"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="P46" s="15" t="s">
+      <c r="P46" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
       <c r="S46" s="5">
         <f ca="1">K44+S44</f>
         <v>108193.64865290908</v>
@@ -4170,9 +4185,9 @@
       <c r="K47" s="5"/>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
       <c r="S47" s="5"/>
     </row>
   </sheetData>
@@ -4206,77 +4221,97 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan3"/>
-  <dimension ref="D6:G12"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
         <v>97</v>
       </c>
-      <c r="F7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D5" t="s">
         <v>98</v>
       </c>
-      <c r="F10" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>99</v>
       </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C7" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>